<commit_message>
synthesize Hollis 2019 data
</commit_message>
<xml_diff>
--- a/data/raw/Eocene/Hollis2019SI/Hollis2019_D47_locations_and_values.xlsx
+++ b/data/raw/Eocene/Hollis2019SI/Hollis2019_D47_locations_and_values.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\PalaeoClimateGradient\data\raw\Eocene\Hollis2019SI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89752E2F-AD93-4D6B-B3D7-B322D29C349A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD9DCDEF-1C96-44A4-90A2-F1DA6261365E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3091D935-901D-4887-B397-A4352051D1D5}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="33">
   <si>
     <t>USA</t>
   </si>
@@ -130,16 +130,20 @@
   </si>
   <si>
     <t>N_replicates</t>
+  </si>
+  <si>
+    <t>D47</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -213,6 +217,11 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -228,7 +237,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -265,11 +274,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -342,6 +360,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -658,10 +688,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B2836B4-D4C2-4500-8989-F059700D00FB}">
-  <dimension ref="A1:O30"/>
+  <dimension ref="A1:P30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -674,7 +704,7 @@
     <col min="7" max="7" width="22.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -720,8 +750,11 @@
       <c r="O1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -764,8 +797,11 @@
       <c r="O2" s="24">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P2" s="26">
+        <v>0.72399999999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -808,8 +844,11 @@
       <c r="O3" s="25">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P3" s="27">
+        <v>0.71699999999999997</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -852,8 +891,11 @@
       <c r="O4" s="24">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P4" s="26">
+        <v>0.68200000000000005</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -896,8 +938,11 @@
       <c r="O5" s="24">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P5" s="28">
+        <v>0.67300000000000004</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -940,8 +985,11 @@
       <c r="O6" s="24">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P6" s="29">
+        <v>0.65700000000000003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -984,8 +1032,11 @@
       <c r="O7" s="24">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P7" s="26">
+        <v>0.63800000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -1028,41 +1079,44 @@
       <c r="O8" s="24">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P8" s="28">
+        <v>0.63400000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="F9" s="3"/>
       <c r="G9" s="2"/>
       <c r="L9" s="14"/>
       <c r="M9" s="15"/>
       <c r="N9" s="16"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="F11" s="6"/>
       <c r="G11" s="5"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E12" s="8"/>
       <c r="F12" s="1"/>
       <c r="G12" s="7"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E13" s="8"/>
       <c r="F13" s="1"/>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="F14" s="1"/>
       <c r="G14" s="5"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="F15" s="1"/>
       <c r="G15" s="2"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="F16" s="1"/>
       <c r="G16" s="2"/>
     </row>

</xml_diff>